<commit_message>
added overhead data and mont ml
</commit_message>
<xml_diff>
--- a/powerTraces/datapoints/resultsGraph.xlsx
+++ b/powerTraces/datapoints/resultsGraph.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caiju\Documents\ClassDocuments\EE382NEmbeddedSystemDesignAndModeling\SecurityProject\powerTraces\datapoints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvin\Documents\UT Austin\Graduate School\EE382V Security HW SW Interface\research_clean\SecurityProject\powerTraces\datapoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>datapoint12</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t>datapoint29</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>energy-forloopenergy</t>
+  </si>
+  <si>
+    <t>time-forlooptime</t>
+  </si>
+  <si>
+    <t>power for (energy-emptyloop)</t>
   </si>
 </sst>
 </file>
@@ -894,7 +912,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>6</c:v>
@@ -1044,7 +1062,7 @@
                   <c:v>11.6091</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.6968399999999999</c:v>
+                  <c:v>11.0564</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>23.239599999999999</c:v>
@@ -1391,6 +1409,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1398,6 +1417,573 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$F$1:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$E$1:$E$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>55.420400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.719999999999985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.68562000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.613399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.613399999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.297199999999989</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.828898721949997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89.060699999999983</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.559299999999993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55.224600000000009</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>61.500099999999989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61.419800000000009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51.759240000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>61.419800000000009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22.568679999999986</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55.484200000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>67.155180000000016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27.110499999999988</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>69.87939999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>112.7684</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>49.890999999999991</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44.36399999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>73.2376</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>55.297199999999989</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55.224600000000009</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>129.76299999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61.500099999999989</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44.243999999999986</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>103.68562000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>55.224600000000009</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>122.5408</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44.355999999999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>55.224600000000009</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>55.224600000000009</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>133.17663999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44.186000000000007</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>155.14945</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>135.49137999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000008B-A417-4691-B6EC-523A6E7F9DD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="420885288"/>
+        <c:axId val="420885616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="420885288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420885616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="420885616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420885288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1473,7 +2059,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2022,6 +3164,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05033BAA-8C2E-4DCE-B8DC-63D1BF7B311B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2327,18 +3505,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2349,10 +3527,23 @@
         <v>11</v>
       </c>
       <c r="D1">
-        <v>1.00512727273</v>
+        <f>B1*C1</f>
+        <v>121.6204</v>
+      </c>
+      <c r="E1">
+        <f>D1-(6.62*10)</f>
+        <v>55.420400000000001</v>
+      </c>
+      <c r="F1">
+        <f>C1-10</f>
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <f>E1/F1</f>
+        <v>55.420400000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2363,10 +3554,23 @@
         <v>16</v>
       </c>
       <c r="D2">
-        <v>0.62859374999999995</v>
+        <f t="shared" ref="D2:D48" si="0">B2*C2</f>
+        <v>160.91999999999999</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E48" si="1">D2-(6.62*10)</f>
+        <v>94.719999999999985</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F48" si="2">C2-10</f>
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G48" si="3">E2/F2</f>
+        <v>15.786666666666664</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2377,10 +3581,23 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>0.52433833333299995</v>
+        <f t="shared" si="0"/>
+        <v>169.88562000000002</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>103.68562000000001</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="3"/>
+        <v>12.960702500000002</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2391,10 +3608,23 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>1.0563090909099999</v>
+        <f t="shared" si="0"/>
+        <v>127.8134</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>61.613399999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>61.613399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2405,10 +3635,23 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>1.16194</v>
+        <f t="shared" si="0"/>
+        <v>116.194</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>49.994</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2419,10 +3662,23 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>1.0563090909099999</v>
+        <f t="shared" si="0"/>
+        <v>127.8134</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>61.613399999999999</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>61.613399999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2433,10 +3689,23 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>3.7283599999999999</v>
+        <f t="shared" si="0"/>
+        <v>93.209000000000003</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>27.009</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>-5.4017999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2447,10 +3716,23 @@
         <v>11</v>
       </c>
       <c r="D8">
-        <v>1.0041090909099999</v>
+        <f t="shared" si="0"/>
+        <v>121.49719999999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>55.297199999999989</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>55.297199999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2461,10 +3743,23 @@
         <v>43</v>
       </c>
       <c r="D9">
-        <v>5.4098917642999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>100.02889872195</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>33.828898721949997</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>1.0251181430893939</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2475,10 +3770,23 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>3.1685857142899998</v>
+        <f t="shared" si="0"/>
+        <v>155.26069999999999</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>89.060699999999983</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>-29.686899999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2489,10 +3797,23 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2503,10 +3824,23 @@
         <v>7</v>
       </c>
       <c r="D12">
-        <v>3.2399857142899999</v>
+        <f t="shared" si="0"/>
+        <v>158.7593</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>92.559299999999993</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>-30.853099999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2517,10 +3851,23 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <v>1.00350909091</v>
+        <f t="shared" si="0"/>
+        <v>121.42460000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>55.224600000000009</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>55.224600000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2531,10 +3878,23 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>1.05537272727</v>
+        <f t="shared" si="0"/>
+        <v>127.70009999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>61.500099999999989</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>61.500099999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2545,10 +3905,23 @@
         <v>11</v>
       </c>
       <c r="D15">
-        <v>1.0547090909100001</v>
+        <f t="shared" si="0"/>
+        <v>127.61980000000001</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>61.419800000000009</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>61.419800000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2559,10 +3932,23 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G16" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2573,10 +3959,23 @@
         <v>14</v>
       </c>
       <c r="D17">
-        <v>0.60183285714300006</v>
+        <f t="shared" si="0"/>
+        <v>117.95924000000001</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>51.759240000000005</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>12.939810000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2587,10 +3986,23 @@
         <v>11</v>
       </c>
       <c r="D18">
-        <v>1.0547090909100001</v>
+        <f t="shared" si="0"/>
+        <v>127.61980000000001</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>61.419800000000009</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>61.419800000000009</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2601,10 +4013,23 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2615,10 +4040,23 @@
         <v>11</v>
       </c>
       <c r="D20">
-        <v>0.73362545454500006</v>
+        <f t="shared" si="0"/>
+        <v>88.768679999999989</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>22.568679999999986</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>22.568679999999986</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2629,10 +4067,23 @@
         <v>11</v>
       </c>
       <c r="D21">
-        <v>1.0056545454500001</v>
+        <f t="shared" si="0"/>
+        <v>121.6842</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>55.484200000000001</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>55.484200000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2643,10 +4094,23 @@
         <v>14</v>
       </c>
       <c r="D22">
-        <v>0.68038357142899997</v>
+        <f t="shared" si="0"/>
+        <v>133.35518000000002</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>67.155180000000016</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>16.788795000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2657,10 +4121,23 @@
         <v>5</v>
       </c>
       <c r="D23">
-        <v>3.7324199999999998</v>
+        <f t="shared" si="0"/>
+        <v>93.31049999999999</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>27.110499999999988</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>-5.4220999999999977</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2671,10 +4148,23 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <v>3.7799833333300001</v>
+        <f t="shared" si="0"/>
+        <v>136.07939999999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>69.87939999999999</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>-17.469849999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2685,10 +4175,23 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>0.44742100000000001</v>
+        <f t="shared" si="0"/>
+        <v>178.9684</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>112.7684</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>11.27684</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2699,24 +4202,50 @@
         <v>10</v>
       </c>
       <c r="D26">
-        <v>1.1609100000000001</v>
+        <f t="shared" si="0"/>
+        <v>116.09099999999999</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>49.890999999999991</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>9.6968399999999999</v>
+        <v>11.0564</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D27">
-        <v>9.6968399999999999</v>
+        <f t="shared" si="0"/>
+        <v>110.56399999999999</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>44.36399999999999</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G27" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2727,10 +4256,23 @@
         <v>6</v>
       </c>
       <c r="D28">
-        <v>3.8732666666700002</v>
+        <f t="shared" si="0"/>
+        <v>139.4376</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>73.2376</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>-18.3094</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2741,10 +4283,23 @@
         <v>11</v>
       </c>
       <c r="D29">
-        <v>1.0041090909099999</v>
+        <f t="shared" si="0"/>
+        <v>121.49719999999999</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>55.297199999999989</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>55.297199999999989</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2755,10 +4310,23 @@
         <v>11</v>
       </c>
       <c r="D30">
-        <v>1.00350909091</v>
+        <f t="shared" si="0"/>
+        <v>121.42460000000001</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>55.224600000000009</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>55.224600000000009</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2769,10 +4337,23 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>1.95963</v>
+        <f t="shared" si="0"/>
+        <v>195.96299999999999</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>129.76299999999998</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G31" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2783,10 +4364,23 @@
         <v>11</v>
       </c>
       <c r="D32">
-        <v>1.05537272727</v>
+        <f t="shared" si="0"/>
+        <v>127.70009999999999</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>61.500099999999989</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>61.500099999999989</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2797,10 +4391,23 @@
         <v>10</v>
       </c>
       <c r="D33">
-        <v>1.1044400000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.44399999999999</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>44.243999999999986</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G33" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2811,10 +4418,23 @@
         <v>18</v>
       </c>
       <c r="D34">
-        <v>0.52433833333299995</v>
+        <f t="shared" si="0"/>
+        <v>169.88562000000002</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>103.68562000000001</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>12.960702500000002</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2825,10 +4445,23 @@
         <v>11</v>
       </c>
       <c r="D35">
-        <v>1.00350909091</v>
+        <f t="shared" si="0"/>
+        <v>121.42460000000001</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>55.224600000000009</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>55.224600000000009</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2839,10 +4472,23 @@
         <v>9</v>
       </c>
       <c r="D36">
-        <v>2.3301333333300001</v>
+        <f t="shared" si="0"/>
+        <v>188.74080000000001</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>122.5408</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>-122.5408</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2853,10 +4499,23 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G37" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2867,10 +4526,23 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G38" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2881,10 +4553,23 @@
         <v>10</v>
       </c>
       <c r="D39">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2895,10 +4580,23 @@
         <v>10</v>
       </c>
       <c r="D40">
-        <v>1.1055600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.556</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>44.355999999999995</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G40" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2909,10 +4607,23 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G41" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2923,10 +4634,23 @@
         <v>11</v>
       </c>
       <c r="D42">
-        <v>1.00350909091</v>
+        <f t="shared" si="0"/>
+        <v>121.42460000000001</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>55.224600000000009</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="3"/>
+        <v>55.224600000000009</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2937,10 +4661,23 @@
         <v>10</v>
       </c>
       <c r="D43">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G43" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2951,10 +4688,23 @@
         <v>11</v>
       </c>
       <c r="D44">
-        <v>1.00350909091</v>
+        <f t="shared" si="0"/>
+        <v>121.42460000000001</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>55.224600000000009</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="3"/>
+        <v>55.224600000000009</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2965,10 +4715,23 @@
         <v>27</v>
       </c>
       <c r="D45">
-        <v>0.27349333333300002</v>
+        <f t="shared" si="0"/>
+        <v>199.37663999999998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>133.17663999999996</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="3"/>
+        <v>7.8339199999999982</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2979,10 +4742,23 @@
         <v>10</v>
       </c>
       <c r="D46">
-        <v>1.1038600000000001</v>
+        <f t="shared" si="0"/>
+        <v>110.38600000000001</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>44.186000000000007</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G46" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2993,10 +4769,23 @@
         <v>35</v>
       </c>
       <c r="D47">
-        <v>0.18069342857099999</v>
+        <f t="shared" si="0"/>
+        <v>221.34945000000002</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>155.14945</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="3"/>
+        <v>6.205978</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -3007,7 +4796,40 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <v>50.422845000000002</v>
+        <f t="shared" si="0"/>
+        <v>201.69138000000001</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>135.49137999999999</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="3"/>
+        <v>-16.936422499999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>